<commit_message>
Modification de la répartition des heures
</commit_message>
<xml_diff>
--- a/Antoine/Journal_Travail.xlsx
+++ b/Antoine/Journal_Travail.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19029"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Date</t>
   </si>
@@ -36,19 +36,28 @@
     <t>Journal de travail</t>
   </si>
   <si>
-    <t>Albert Einstein</t>
-  </si>
-  <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
-  </si>
-  <si>
-    <t>blablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablablabla</t>
+    <t>Présentation des directives du projet, constitution des groupes et discussion des différentes idées de projet. Au fin de la séance : décision finale de la proposition : BlaajjPaint</t>
+  </si>
+  <si>
+    <t>Relecture et complétion de la proposition à rendre</t>
+  </si>
+  <si>
+    <t>Retour du professeur sur notre proposition de projet et discussion entre l'équipe concernant les dates de rencontres et les fonctionnalités à mettre dans le cahier des charges</t>
+  </si>
+  <si>
+    <t>Rédaction et discussion sur le cahier des charges ainsi que début de conception du diagramme de Gantt et répartition des heures</t>
+  </si>
+  <si>
+    <t>Réunion du groupe afin de discuter des souhaits de chacun, des spécificités du projets et des fonctionnalités (générales ou optionnelles). Conception également d'un schéma de dépendances fonctionnelles afin de faciliter le futur diagramme de Gantt</t>
+  </si>
+  <si>
+    <t>Antoine Rochat</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd/mm/yy;@"/>
   </numFmts>
@@ -439,33 +448,33 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="52.5546875" customWidth="1"/>
+    <col min="2" max="2" width="52.53125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" s="6" customFormat="1" ht="25.5" x14ac:dyDescent="0.75">
       <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" ht="23.25" x14ac:dyDescent="0.7">
       <c r="A2" s="10" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
     </row>
-    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
         <v>0</v>
       </c>
@@ -476,160 +485,178 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="44.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>43150</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="3">
+        <v>43153</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="8">
-        <v>1.25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="3">
-        <v>43152</v>
-      </c>
-      <c r="B6" s="4" t="s">
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A7" s="3">
+        <v>43157</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="8">
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="8"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="8"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="8"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C7" s="8">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="A8" s="3">
+        <v>43158</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A9" s="3">
+        <v>43161</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="3"/>
       <c r="B11" s="4"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="3"/>
       <c r="B12" s="4"/>
       <c r="C12" s="8"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="3"/>
       <c r="B13" s="4"/>
       <c r="C13" s="8"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="3"/>
       <c r="B14" s="4"/>
       <c r="C14" s="8"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="3"/>
       <c r="B15" s="4"/>
       <c r="C15" s="8"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="3"/>
       <c r="B16" s="4"/>
       <c r="C16" s="8"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="3"/>
       <c r="B17" s="4"/>
       <c r="C17" s="8"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="3"/>
       <c r="B18" s="4"/>
       <c r="C18" s="8"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="3"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="3"/>
       <c r="B21" s="4"/>
       <c r="C21" s="8"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="3"/>
       <c r="B22" s="4"/>
       <c r="C22" s="8"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="3"/>
       <c r="B23" s="4"/>
       <c r="C23" s="8"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="3"/>
       <c r="B24" s="4"/>
       <c r="C24" s="8"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="3"/>
       <c r="B25" s="4"/>
       <c r="C25" s="8"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="3"/>
       <c r="B26" s="4"/>
       <c r="C26" s="8"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="3"/>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="3"/>
       <c r="B29" s="4"/>
       <c r="C29" s="8"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="3"/>
       <c r="B30" s="4"/>
       <c r="C30" s="8"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.45">
       <c r="B32" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C32" s="9">
         <f>SUM(C5:C31)</f>
-        <v>3</v>
+        <v>10.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>